<commit_message>
neu: Anzahl Kinder, Familien
</commit_message>
<xml_diff>
--- a/data/GedCom.xlsx
+++ b/data/GedCom.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfg\Desktop\Ahnen und R\GitHub_neu\ahnen-main\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfg\HiDrive\Rike R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A5B729-4E6F-4ACF-BB86-7834A842AE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7B94ACA-658F-4ED2-89F6-40977514E740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{DDA6A7E4-9F3E-4282-89E4-7587E2E1C520}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="203">
   <si>
     <t>NAME_1</t>
   </si>
@@ -631,6 +631,18 @@
   </si>
   <si>
     <t>TODESURSACHE</t>
+  </si>
+  <si>
+    <t>FAMILIE_1</t>
+  </si>
+  <si>
+    <t>FAMILIE_2</t>
+  </si>
+  <si>
+    <t>FAMILIE_3</t>
+  </si>
+  <si>
+    <t>FAMILIE_4</t>
   </si>
 </sst>
 </file>
@@ -1025,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA657514-F280-46FB-9B4A-D41649D1C321}">
   <dimension ref="A1:C169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -1620,7 +1632,9 @@
       <c r="B59" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="4"/>
+      <c r="C59" s="4" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60" s="7">
@@ -1629,7 +1643,9 @@
       <c r="B60" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="4"/>
+      <c r="C60" s="4" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61" s="7">
@@ -1638,7 +1654,9 @@
       <c r="B61" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="4"/>
+      <c r="C61" s="4" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A62" s="7">
@@ -1647,7 +1665,9 @@
       <c r="B62" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="4"/>
+      <c r="C62" s="4" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A63" s="7">

</xml_diff>

<commit_message>
Anzahl Kinder + Stammbäume
</commit_message>
<xml_diff>
--- a/data/GedCom.xlsx
+++ b/data/GedCom.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfg\HiDrive\Rike R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uniem\Documents\_Git\ahnen_v\ahnen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7B94ACA-658F-4ED2-89F6-40977514E740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFAA9FF-F4BC-4D97-951C-417071CAD8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{DDA6A7E4-9F3E-4282-89E4-7587E2E1C520}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{DDA6A7E4-9F3E-4282-89E4-7587E2E1C520}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
   <si>
     <t>NAME_1</t>
   </si>
@@ -549,9 +550,6 @@
     <t>SpaltenNr</t>
   </si>
   <si>
-    <t>KONFIRMATIONSORT</t>
-  </si>
-  <si>
     <t>TODESORT</t>
   </si>
   <si>
@@ -567,39 +565,9 @@
     <t>BERUF</t>
   </si>
   <si>
-    <t>GENERATION</t>
-  </si>
-  <si>
-    <t>QUELLEN</t>
-  </si>
-  <si>
     <t>GESCHLECHT</t>
   </si>
   <si>
-    <t>KONFIRMATIONSDATUM</t>
-  </si>
-  <si>
-    <t>KONF_GEO_BREITE</t>
-  </si>
-  <si>
-    <t>KONF_GEO_LAENGE</t>
-  </si>
-  <si>
-    <t>TAUFORT</t>
-  </si>
-  <si>
-    <t>TAUFDATUM</t>
-  </si>
-  <si>
-    <t>BO_GEO_BREITE</t>
-  </si>
-  <si>
-    <t>BO_GEO_LAENGE</t>
-  </si>
-  <si>
-    <t>BEGRAEBNISORT</t>
-  </si>
-  <si>
     <t>GEBURTSDATUM</t>
   </si>
   <si>
@@ -612,9 +580,6 @@
     <t>GO_GEO_LAENGE</t>
   </si>
   <si>
-    <t>RUFNAME</t>
-  </si>
-  <si>
     <t>NACHNAME</t>
   </si>
   <si>
@@ -627,9 +592,6 @@
     <t>TODESDATUM</t>
   </si>
   <si>
-    <t>BEGRAEBNISDATUM</t>
-  </si>
-  <si>
     <t>TODESURSACHE</t>
   </si>
   <si>
@@ -643,6 +605,9 @@
   </si>
   <si>
     <t>FAMILIE_4</t>
+  </si>
+  <si>
+    <t>ELTERN</t>
   </si>
 </sst>
 </file>
@@ -671,12 +636,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -706,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -721,6 +692,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -739,9 +711,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -779,7 +751,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -885,7 +857,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1027,7 +999,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1037,19 +1009,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA657514-F280-46FB-9B4A-D41649D1C321}">
   <dimension ref="A1:C169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148:C148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="2"/>
-    <col min="2" max="2" width="39.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.1328125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="1" width="10.7109375" style="2"/>
+    <col min="2" max="2" width="39.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>170</v>
       </c>
@@ -1060,7 +1032,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1068,10 +1040,10 @@
         <v>169</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1080,7 +1052,7 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1088,10 +1060,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1100,7 +1072,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1109,7 +1081,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1117,10 +1089,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1129,18 +1101,16 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1149,7 +1119,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1158,7 +1128,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1167,7 +1137,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1176,7 +1146,7 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1184,10 +1154,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1196,7 +1166,7 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -1204,10 +1174,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1215,10 +1185,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -1226,10 +1196,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1238,7 +1208,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -1247,18 +1217,16 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1267,40 +1235,34 @@
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -1309,7 +1271,7 @@
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -1318,7 +1280,7 @@
       </c>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -1327,7 +1289,7 @@
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -1336,7 +1298,7 @@
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -1345,51 +1307,43 @@
       </c>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -1398,7 +1352,7 @@
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -1407,7 +1361,7 @@
       </c>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -1416,7 +1370,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -1425,7 +1379,7 @@
       </c>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -1434,18 +1388,16 @@
       </c>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -1454,40 +1406,34 @@
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -1496,7 +1442,7 @@
       </c>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -1505,7 +1451,7 @@
       </c>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -1514,7 +1460,7 @@
       </c>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -1523,7 +1469,7 @@
       </c>
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -1531,10 +1477,10 @@
         <v>46</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -1542,10 +1488,10 @@
         <v>47</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -1554,7 +1500,7 @@
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -1562,10 +1508,10 @@
         <v>49</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -1573,10 +1519,10 @@
         <v>50</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -1584,10 +1530,10 @@
         <v>51</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>54</v>
       </c>
@@ -1596,7 +1542,7 @@
       </c>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -1604,10 +1550,10 @@
         <v>53</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -1616,16 +1562,18 @@
       </c>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="4"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C58" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -1633,10 +1581,10 @@
         <v>56</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -1644,10 +1592,10 @@
         <v>57</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>60</v>
       </c>
@@ -1655,10 +1603,10 @@
         <v>58</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -1666,10 +1614,10 @@
         <v>59</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -1678,7 +1626,7 @@
       </c>
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -1687,7 +1635,7 @@
       </c>
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>64</v>
       </c>
@@ -1696,7 +1644,7 @@
       </c>
       <c r="C65" s="4"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>65</v>
       </c>
@@ -1705,7 +1653,7 @@
       </c>
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -1714,7 +1662,7 @@
       </c>
       <c r="C67" s="4"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -1723,7 +1671,7 @@
       </c>
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -1732,7 +1680,7 @@
       </c>
       <c r="C69" s="4"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -1741,7 +1689,7 @@
       </c>
       <c r="C70" s="4"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
         <v>70</v>
       </c>
@@ -1750,7 +1698,7 @@
       </c>
       <c r="C71" s="4"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
         <v>71</v>
       </c>
@@ -1759,7 +1707,7 @@
       </c>
       <c r="C72" s="4"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
         <v>72</v>
       </c>
@@ -1768,7 +1716,7 @@
       </c>
       <c r="C73" s="4"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
         <v>73</v>
       </c>
@@ -1777,7 +1725,7 @@
       </c>
       <c r="C74" s="4"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
         <v>74</v>
       </c>
@@ -1786,7 +1734,7 @@
       </c>
       <c r="C75" s="4"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
         <v>75</v>
       </c>
@@ -1795,7 +1743,7 @@
       </c>
       <c r="C76" s="4"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
         <v>76</v>
       </c>
@@ -1804,7 +1752,7 @@
       </c>
       <c r="C77" s="4"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
         <v>77</v>
       </c>
@@ -1813,7 +1761,7 @@
       </c>
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
         <v>78</v>
       </c>
@@ -1822,7 +1770,7 @@
       </c>
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
         <v>79</v>
       </c>
@@ -1831,7 +1779,7 @@
       </c>
       <c r="C80" s="4"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
         <v>80</v>
       </c>
@@ -1840,7 +1788,7 @@
       </c>
       <c r="C81" s="4"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
         <v>81</v>
       </c>
@@ -1849,7 +1797,7 @@
       </c>
       <c r="C82" s="4"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
         <v>82</v>
       </c>
@@ -1858,7 +1806,7 @@
       </c>
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>83</v>
       </c>
@@ -1867,7 +1815,7 @@
       </c>
       <c r="C84" s="4"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
         <v>84</v>
       </c>
@@ -1876,7 +1824,7 @@
       </c>
       <c r="C85" s="4"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
         <v>85</v>
       </c>
@@ -1885,7 +1833,7 @@
       </c>
       <c r="C86" s="4"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
         <v>86</v>
       </c>
@@ -1894,7 +1842,7 @@
       </c>
       <c r="C87" s="4"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
         <v>87</v>
       </c>
@@ -1903,7 +1851,7 @@
       </c>
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
         <v>88</v>
       </c>
@@ -1912,7 +1860,7 @@
       </c>
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
         <v>89</v>
       </c>
@@ -1921,7 +1869,7 @@
       </c>
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
         <v>90</v>
       </c>
@@ -1930,7 +1878,7 @@
       </c>
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
         <v>91</v>
       </c>
@@ -1939,7 +1887,7 @@
       </c>
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -1948,7 +1896,7 @@
       </c>
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
         <v>93</v>
       </c>
@@ -1957,7 +1905,7 @@
       </c>
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
         <v>94</v>
       </c>
@@ -1966,7 +1914,7 @@
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
         <v>95</v>
       </c>
@@ -1975,7 +1923,7 @@
       </c>
       <c r="C96" s="4"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="7">
         <v>96</v>
       </c>
@@ -1984,7 +1932,7 @@
       </c>
       <c r="C97" s="4"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
         <v>97</v>
       </c>
@@ -1993,7 +1941,7 @@
       </c>
       <c r="C98" s="4"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
         <v>98</v>
       </c>
@@ -2002,7 +1950,7 @@
       </c>
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
         <v>99</v>
       </c>
@@ -2011,7 +1959,7 @@
       </c>
       <c r="C100" s="4"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
         <v>100</v>
       </c>
@@ -2020,7 +1968,7 @@
       </c>
       <c r="C101" s="4"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
         <v>101</v>
       </c>
@@ -2029,7 +1977,7 @@
       </c>
       <c r="C102" s="4"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
         <v>102</v>
       </c>
@@ -2038,7 +1986,7 @@
       </c>
       <c r="C103" s="4"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
         <v>103</v>
       </c>
@@ -2047,7 +1995,7 @@
       </c>
       <c r="C104" s="4"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
         <v>104</v>
       </c>
@@ -2056,7 +2004,7 @@
       </c>
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
         <v>105</v>
       </c>
@@ -2065,7 +2013,7 @@
       </c>
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
         <v>106</v>
       </c>
@@ -2074,7 +2022,7 @@
       </c>
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
         <v>107</v>
       </c>
@@ -2083,7 +2031,7 @@
       </c>
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
         <v>108</v>
       </c>
@@ -2092,7 +2040,7 @@
       </c>
       <c r="C109" s="4"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
         <v>109</v>
       </c>
@@ -2101,7 +2049,7 @@
       </c>
       <c r="C110" s="4"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="7">
         <v>110</v>
       </c>
@@ -2110,7 +2058,7 @@
       </c>
       <c r="C111" s="4"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
         <v>111</v>
       </c>
@@ -2119,7 +2067,7 @@
       </c>
       <c r="C112" s="4"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
         <v>112</v>
       </c>
@@ -2128,7 +2076,7 @@
       </c>
       <c r="C113" s="4"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
         <v>113</v>
       </c>
@@ -2137,7 +2085,7 @@
       </c>
       <c r="C114" s="4"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="7">
         <v>114</v>
       </c>
@@ -2146,7 +2094,7 @@
       </c>
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="7">
         <v>115</v>
       </c>
@@ -2155,7 +2103,7 @@
       </c>
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="7">
         <v>116</v>
       </c>
@@ -2164,7 +2112,7 @@
       </c>
       <c r="C117" s="4"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="7">
         <v>117</v>
       </c>
@@ -2173,7 +2121,7 @@
       </c>
       <c r="C118" s="4"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
         <v>118</v>
       </c>
@@ -2182,7 +2130,7 @@
       </c>
       <c r="C119" s="4"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
         <v>119</v>
       </c>
@@ -2191,7 +2139,7 @@
       </c>
       <c r="C120" s="4"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="7">
         <v>120</v>
       </c>
@@ -2200,7 +2148,7 @@
       </c>
       <c r="C121" s="4"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
         <v>121</v>
       </c>
@@ -2209,7 +2157,7 @@
       </c>
       <c r="C122" s="4"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
         <v>122</v>
       </c>
@@ -2218,7 +2166,7 @@
       </c>
       <c r="C123" s="4"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
         <v>123</v>
       </c>
@@ -2227,7 +2175,7 @@
       </c>
       <c r="C124" s="4"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="7">
         <v>124</v>
       </c>
@@ -2236,7 +2184,7 @@
       </c>
       <c r="C125" s="4"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="7">
         <v>125</v>
       </c>
@@ -2245,7 +2193,7 @@
       </c>
       <c r="C126" s="4"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
         <v>126</v>
       </c>
@@ -2254,7 +2202,7 @@
       </c>
       <c r="C127" s="4"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="7">
         <v>127</v>
       </c>
@@ -2263,7 +2211,7 @@
       </c>
       <c r="C128" s="4"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
         <v>128</v>
       </c>
@@ -2272,7 +2220,7 @@
       </c>
       <c r="C129" s="4"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="7">
         <v>129</v>
       </c>
@@ -2281,7 +2229,7 @@
       </c>
       <c r="C130" s="4"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
         <v>130</v>
       </c>
@@ -2290,7 +2238,7 @@
       </c>
       <c r="C131" s="4"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="7">
         <v>131</v>
       </c>
@@ -2299,7 +2247,7 @@
       </c>
       <c r="C132" s="4"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="7">
         <v>132</v>
       </c>
@@ -2308,7 +2256,7 @@
       </c>
       <c r="C133" s="4"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="7">
         <v>133</v>
       </c>
@@ -2317,7 +2265,7 @@
       </c>
       <c r="C134" s="4"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="7">
         <v>134</v>
       </c>
@@ -2326,7 +2274,7 @@
       </c>
       <c r="C135" s="4"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="7">
         <v>135</v>
       </c>
@@ -2335,7 +2283,7 @@
       </c>
       <c r="C136" s="4"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="7">
         <v>136</v>
       </c>
@@ -2344,7 +2292,7 @@
       </c>
       <c r="C137" s="4"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="7">
         <v>137</v>
       </c>
@@ -2353,7 +2301,7 @@
       </c>
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="7">
         <v>138</v>
       </c>
@@ -2361,10 +2309,10 @@
         <v>136</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="7">
         <v>139</v>
       </c>
@@ -2373,7 +2321,7 @@
       </c>
       <c r="C140" s="4"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="7">
         <v>140</v>
       </c>
@@ -2382,7 +2330,7 @@
       </c>
       <c r="C141" s="4"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="7">
         <v>141</v>
       </c>
@@ -2391,7 +2339,7 @@
       </c>
       <c r="C142" s="4"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="7">
         <v>142</v>
       </c>
@@ -2400,7 +2348,7 @@
       </c>
       <c r="C143" s="4"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="7">
         <v>143</v>
       </c>
@@ -2409,7 +2357,7 @@
       </c>
       <c r="C144" s="4"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="7">
         <v>144</v>
       </c>
@@ -2418,7 +2366,7 @@
       </c>
       <c r="C145" s="4"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="7">
         <v>145</v>
       </c>
@@ -2427,7 +2375,7 @@
       </c>
       <c r="C146" s="4"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="7">
         <v>146</v>
       </c>
@@ -2436,18 +2384,16 @@
       </c>
       <c r="C147" s="4"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="7">
         <v>147</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C148" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C148" s="8"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="7">
         <v>148</v>
       </c>
@@ -2456,7 +2402,7 @@
       </c>
       <c r="C149" s="4"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="7">
         <v>149</v>
       </c>
@@ -2465,7 +2411,7 @@
       </c>
       <c r="C150" s="4"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="7">
         <v>150</v>
       </c>
@@ -2474,7 +2420,7 @@
       </c>
       <c r="C151" s="4"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="7">
         <v>151</v>
       </c>
@@ -2482,21 +2428,19 @@
         <v>149</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="7">
         <v>152</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C153" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C153" s="4"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="7">
         <v>153</v>
       </c>
@@ -2505,7 +2449,7 @@
       </c>
       <c r="C154" s="4"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="7">
         <v>154</v>
       </c>
@@ -2514,7 +2458,7 @@
       </c>
       <c r="C155" s="4"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
         <v>155</v>
       </c>
@@ -2523,7 +2467,7 @@
       </c>
       <c r="C156" s="4"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="7">
         <v>156</v>
       </c>
@@ -2532,7 +2476,7 @@
       </c>
       <c r="C157" s="4"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="7">
         <v>157</v>
       </c>
@@ -2541,7 +2485,7 @@
       </c>
       <c r="C158" s="4"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="7">
         <v>158</v>
       </c>
@@ -2550,7 +2494,7 @@
       </c>
       <c r="C159" s="4"/>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="7">
         <v>159</v>
       </c>
@@ -2559,7 +2503,7 @@
       </c>
       <c r="C160" s="4"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="7">
         <v>160</v>
       </c>
@@ -2568,7 +2512,7 @@
       </c>
       <c r="C161" s="4"/>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="7">
         <v>161</v>
       </c>
@@ -2577,7 +2521,7 @@
       </c>
       <c r="C162" s="4"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="7">
         <v>162</v>
       </c>
@@ -2586,7 +2530,7 @@
       </c>
       <c r="C163" s="4"/>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="7">
         <v>163</v>
       </c>
@@ -2595,7 +2539,7 @@
       </c>
       <c r="C164" s="4"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="7">
         <v>164</v>
       </c>
@@ -2604,7 +2548,7 @@
       </c>
       <c r="C165" s="4"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="7">
         <v>165</v>
       </c>
@@ -2613,7 +2557,7 @@
       </c>
       <c r="C166" s="4"/>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="7">
         <v>166</v>
       </c>
@@ -2622,7 +2566,7 @@
       </c>
       <c r="C167" s="4"/>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="7">
         <v>167</v>
       </c>
@@ -2631,7 +2575,7 @@
       </c>
       <c r="C168" s="4"/>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="7">
         <v>168</v>
       </c>
@@ -2644,4 +2588,16 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730BE51D-041C-4250-BD70-0CEB4205B8D0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>